<commit_message>
done dev add single formula
</commit_message>
<xml_diff>
--- a/test_formula.xlsx
+++ b/test_formula.xlsx
@@ -1,75 +1,83 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <x:workbookPr/>
+  <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Csharp\excelExport\"/>
+  <x:bookViews>
+    <x:workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:calcPr calcId="162913" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
+<file path=xl/calcChain2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:calcChain xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:c r="C1" i="1" l="1"/>
+  <x:c r="D1" i="1" l="1"/>
+</x:calcChain>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:fonts count="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </x:cellStyleXfs>
+  <x:cellXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:dxfs count="0"/>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -330,13 +338,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:dimension ref="A1:B4"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="B5" sqref="B5"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:2">
+      <x:c r="A1">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B1">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C1">
+        <x:f>SUM(A1,B1)</x:f>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="D1">
+        <x:f>SUM(A1,B1)/7+A1</x:f>
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:2">
+      <x:c r="A2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:2">
+      <x:c r="A3">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B3">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:2">
+      <x:c r="A4">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B4">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
done add formula chain
</commit_message>
<xml_diff>
--- a/test_formula.xlsx
+++ b/test_formula.xlsx
@@ -23,6 +23,11 @@
 <x:calcChain xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:c r="C1" i="1" l="1"/>
   <x:c r="D1" i="1" l="1"/>
+  <x:c r="D1" i="1" l="1"/>
+  <x:c r="D2" i="1"/>
+  <x:c r="D3" i="1"/>
+  <x:c r="D4" i="1"/>
+  <x:c r="D5" i="1"/>
 </x:calcChain>
 </file>
 
@@ -370,6 +375,10 @@
       <x:c r="B2">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D2">
+        <x:f t="shared" ref="D2:D5" si="1">SUM(A2,B2)/7+A2</x:f>
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
       <x:c r="A3">
@@ -378,6 +387,10 @@
       <x:c r="B3">
         <x:v>6</x:v>
       </x:c>
+      <x:c r="D3">
+        <x:f t="shared" si="1"/>
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
       <x:c r="A4">
@@ -385,6 +398,16 @@
       </x:c>
       <x:c r="B4">
         <x:v>4</x:v>
+      </x:c>
+      <x:c r="D4">
+        <x:f t="shared" si="1"/>
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5">
+      <x:c r="D5">
+        <x:f t="shared" si="1"/>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>